<commit_message>
Planning few little changes
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\universiteit\jaar 3\kwartiel 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rutger/Desktop/Module 10/Java/Workspace/SSProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,27 +38,6 @@
     <t>Peer feedback</t>
   </si>
   <si>
-    <t>woensdag</t>
-  </si>
-  <si>
-    <t>dinsdag</t>
-  </si>
-  <si>
-    <t>maandag</t>
-  </si>
-  <si>
-    <t>donderdag</t>
-  </si>
-  <si>
-    <t>vrijdag</t>
-  </si>
-  <si>
-    <t>zaterdag</t>
-  </si>
-  <si>
-    <t>zondag</t>
-  </si>
-  <si>
     <t>week 7</t>
   </si>
   <si>
@@ -102,12 +84,33 @@
   </si>
   <si>
     <t>Report</t>
+  </si>
+  <si>
+    <t>wo</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>vr</t>
+  </si>
+  <si>
+    <t>za</t>
+  </si>
+  <si>
+    <t>zo</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>di</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,7 +239,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -248,25 +251,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -275,11 +278,11 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -315,9 +318,10 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,120 +635,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
-    <col min="14" max="14" width="9.140625" style="4"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
-    <col min="26" max="26" width="9.140625" style="4"/>
+    <col min="1" max="1" width="15.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="V2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W2" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="B3" s="5">
         <v>42380</v>
@@ -820,17 +826,17 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -838,9 +844,9 @@
       <c r="K5" s="16"/>
       <c r="Q5" s="16"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -849,18 +855,18 @@
       <c r="N6" s="14"/>
       <c r="Q6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N7" s="24"/>
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q8" s="26"/>
       <c r="R8" s="26"/>
@@ -870,9 +876,9 @@
       <c r="V8" s="26"/>
       <c r="W8" s="26"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
@@ -888,9 +894,9 @@
       <c r="W9" s="22"/>
       <c r="X9" s="21"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -906,9 +912,9 @@
       <c r="W10" s="23"/>
       <c r="X10" s="20"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
@@ -924,13 +930,13 @@
       <c r="W11" s="19"/>
       <c r="X11" s="20"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>2</v>
       </c>
@@ -939,13 +945,13 @@
       <c r="O13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>1</v>
       </c>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>0</v>
       </c>

</xml_diff>